<commit_message>
plot sankey AV-faciliated transformations
</commit_message>
<xml_diff>
--- a/market_assessment.xlsx
+++ b/market_assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/work/Projects/AV Outlook US/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959FEB14-04EA-7743-BEE1-42BBDFE70A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3DBBAC-E249-0C4D-B959-18D0BFDA521D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33680" windowHeight="14260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33680" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US_market_size" sheetId="1" r:id="rId1"/>
@@ -154,14 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -507,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -819,7 +818,7 @@
       <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -857,16 +856,16 @@
       <c r="E2" s="2">
         <v>3.5112359550562302</v>
       </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <f>C2-D2</f>
         <v>233.84831460674081</v>
       </c>
@@ -894,27 +893,27 @@
         <f>C2</f>
         <v>249.29775280898801</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <f>I2/O2 * 100</f>
         <v>93.80281690140842</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="4">
         <f>J2/O2*100</f>
         <v>4.7887323943661944</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="4">
         <f>K2/O2*100</f>
         <v>1.4084507042253767</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="4">
         <f>L2/O2*100</f>
         <v>0</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="4">
         <f>M2/O2*100</f>
         <v>0</v>
       </c>
-      <c r="U2" s="5">
+      <c r="U2" s="4">
         <f>N2/O2*100</f>
         <v>0</v>
       </c>
@@ -935,16 +934,16 @@
       <c r="E3" s="2">
         <v>19.662921348314601</v>
       </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
         <f t="shared" ref="I3:I9" si="0">C3-D3</f>
         <v>183.98876404494359</v>
       </c>
@@ -972,27 +971,27 @@
         <f t="shared" ref="O3:O9" si="6">C3</f>
         <v>250.702247191011</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <f t="shared" ref="P3:P9" si="7">I3/O3 * 100</f>
         <v>73.3893557422969</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="4">
         <f t="shared" ref="Q3:Q9" si="8">J3/O3*100</f>
         <v>18.767507002801135</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="4">
         <f t="shared" ref="R3:R9" si="9">K3/O3*100</f>
         <v>7.8431372549019667</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="4">
         <f t="shared" ref="S3:S9" si="10">L3/O3*100</f>
         <v>0</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="4">
         <f t="shared" ref="T3:T9" si="11">M3/O3*100</f>
         <v>0</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3" s="4">
         <f t="shared" ref="U3:U9" si="12">N3/O3*100</f>
         <v>0</v>
       </c>
@@ -1016,13 +1015,13 @@
       <c r="F4" s="2">
         <v>2.8089887640449498</v>
       </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
         <f t="shared" si="0"/>
         <v>107.02247191011202</v>
       </c>
@@ -1050,27 +1049,27 @@
         <f t="shared" si="6"/>
         <v>257.02247191011202</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="4">
         <f t="shared" si="7"/>
         <v>41.639344262295005</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="4">
         <f t="shared" si="8"/>
         <v>36.502732240437204</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="4">
         <f t="shared" si="9"/>
         <v>20.765027322404407</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="4">
         <f t="shared" si="10"/>
         <v>1.0928961748633919</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -1097,10 +1096,10 @@
       <c r="G5" s="2">
         <v>0.70224719101122401</v>
       </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
         <v>60.34269662921298</v>
       </c>
@@ -1128,27 +1127,27 @@
         <f t="shared" si="6"/>
         <v>263.34269662921298</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="4">
         <f t="shared" si="7"/>
         <v>22.914133333333186</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="4">
         <f t="shared" si="8"/>
         <v>41.61920000000007</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="4">
         <f t="shared" si="9"/>
         <v>32.800000000000075</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="4">
         <f t="shared" si="10"/>
         <v>2.4000000000000057</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5" s="4">
         <f t="shared" si="11"/>
         <v>0.26666666666666261</v>
       </c>
-      <c r="U5" s="5">
+      <c r="U5" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -1178,7 +1177,7 @@
       <c r="H6" s="2">
         <v>0.70224719101122401</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <f t="shared" si="0"/>
         <v>24.578651685392998</v>
       </c>
@@ -1206,27 +1205,27 @@
         <f t="shared" si="6"/>
         <v>269.662921348314</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="4">
         <f t="shared" si="7"/>
         <v>9.1145833333332575</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="4">
         <f t="shared" si="8"/>
         <v>40.104166666666636</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="4">
         <f t="shared" si="9"/>
         <v>38.281250000000085</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="4">
         <f t="shared" si="10"/>
         <v>9.6354166666666625</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="4">
         <f t="shared" si="11"/>
         <v>2.6041666666666932</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6" s="4">
         <f t="shared" si="12"/>
         <v>0.26041666666666285</v>
       </c>
@@ -1256,7 +1255,7 @@
       <c r="H7" s="2">
         <v>4.9157303370786201</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
         <v>9.1292134831460316</v>
       </c>
@@ -1284,27 +1283,27 @@
         <f t="shared" si="6"/>
         <v>271.76966292134802</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="4">
         <f t="shared" si="7"/>
         <v>3.3591731266149774</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="4">
         <f t="shared" si="8"/>
         <v>32.55813953488385</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="4">
         <f t="shared" si="9"/>
         <v>36.69250645994817</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="4">
         <f t="shared" si="10"/>
         <v>18.863049095607245</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="4">
         <f t="shared" si="11"/>
         <v>6.7183462532299982</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="4">
         <f t="shared" si="12"/>
         <v>1.8087855297157527</v>
       </c>
@@ -1334,7 +1333,7 @@
       <c r="H8" s="2">
         <v>13.3426966292134</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>2.8089887640450115</v>
       </c>
@@ -1362,27 +1361,27 @@
         <f t="shared" si="6"/>
         <v>273.17415730337001</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="4">
         <f t="shared" si="7"/>
         <v>1.0282776349614673</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="4">
         <f t="shared" si="8"/>
         <v>22.365038560411186</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="4">
         <f t="shared" si="9"/>
         <v>31.362467866324074</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="4">
         <f t="shared" si="10"/>
         <v>25.706940874035883</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="4">
         <f t="shared" si="11"/>
         <v>14.652956298200573</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="4">
         <f t="shared" si="12"/>
         <v>4.884318766066821</v>
       </c>
@@ -1412,7 +1411,7 @@
       <c r="H9" s="2">
         <v>30.196629213483099</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <f t="shared" si="0"/>
         <v>2.8089887640450115</v>
       </c>
@@ -1440,27 +1439,27 @@
         <f t="shared" si="6"/>
         <v>274.57865168539303</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="4">
         <f t="shared" si="7"/>
         <v>1.0230179028133248</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9" s="4">
         <f t="shared" si="8"/>
         <v>13.810741687979647</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="4">
         <f t="shared" si="9"/>
         <v>24.296675191815726</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="4">
         <f t="shared" si="10"/>
         <v>25.57544757033244</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T9" s="4">
         <f t="shared" si="11"/>
         <v>24.296675191815904</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9" s="4">
         <f t="shared" si="12"/>
         <v>10.997442455242959</v>
       </c>
@@ -1481,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BC560E-917C-BF42-8415-36B25345B8F4}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1526,19 +1525,19 @@
       <c r="A2">
         <v>2015</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>49.236075007849799</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>74.549113875834493</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>99.583987481533697</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>100</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>100</v>
       </c>
       <c r="G2">
@@ -1566,19 +1565,19 @@
       <c r="A3">
         <v>2020</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>33.678483371338302</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>52.593309415101402</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>84.025572261714203</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>99.723070112676496</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>100</v>
       </c>
       <c r="G3">
@@ -1606,19 +1605,19 @@
       <c r="A4">
         <v>2025</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>18.966917687995799</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>30.0922928044556</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>60.272400179129399</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>81.412548321176899</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>100</v>
       </c>
       <c r="G4">
@@ -1646,19 +1645,19 @@
       <c r="A5">
         <v>2030</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>8.8430198740947095</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>14.406325119805601</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>33.5997282175084</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>47.924415641906002</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>100</v>
       </c>
       <c r="G5">
@@ -1686,19 +1685,19 @@
       <c r="A6">
         <v>2035</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>2.8920127861308802</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>5.5345827778435499</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>13.880364229717999</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>20.138259047834801</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>100</v>
       </c>
       <c r="G6">
@@ -1726,19 +1725,19 @@
       <c r="A7">
         <v>2040</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>0.13743546452671801</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.97151945972936504</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>4.0317491365243798</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>6.5356482887483196</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>100</v>
       </c>
       <c r="G7">

</xml_diff>